<commit_message>
2021.04.05 time stamp 13:07
</commit_message>
<xml_diff>
--- a/myData.xlsx
+++ b/myData.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="ม.4 ทั้งหมด" sheetId="1" r:id="rId4"/>
+    <sheet name="ม.4 วิทย์ฯ-คอมฯ" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>เลขที่</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>เลขที่ห้องสอบ</t>
+  </si>
+  <si>
+    <t>4444444444444</t>
+  </si>
+  <si>
+    <t>ม.4</t>
+  </si>
+  <si>
+    <t>นาย</t>
+  </si>
+  <si>
+    <t>วิทย์คอม1</t>
+  </si>
+  <si>
+    <t>วิทยาศาสตร์-คอมพิวเตอร์</t>
+  </si>
+  <si>
+    <t>วิทยาศาสตร์-คณิตศาสตร์</t>
+  </si>
+  <si>
+    <t>อังกฤษ-จีน</t>
+  </si>
+  <si>
+    <t>โรงเรียนธาตุนารายณ์วิทยา</t>
+  </si>
+  <si>
+    <t>0868525525</t>
+  </si>
+  <si>
+    <t>3 มีนาคม 2563</t>
   </si>
 </sst>
 </file>
@@ -423,7 +453,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
@@ -434,20 +464,20 @@
     <col min="3" max="3" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="29.421387" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="10.568848" bestFit="true" customWidth="true" style="0"/>
@@ -524,6 +554,59 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>